<commit_message>
4 Bölümün cetvel de yoksa devam etme özelliği eklendi.
</commit_message>
<xml_diff>
--- a/Config_and_Inputs/ConfigFile.xlsx
+++ b/Config_and_Inputs/ConfigFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\can.sarihan\Documents\UiPath\Taslama_Surec_Otomasyonu\Config_and_Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3595C0-76A7-4235-A6DB-9EC0056C5F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FA6709-008C-40A6-B192-580561C31E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -641,7 +641,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="2">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -652,7 +652,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="3">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -663,7 +663,7 @@
         <v>43</v>
       </c>
       <c r="B11" s="2">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -674,7 +674,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="3">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -684,9 +684,7 @@
       <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="2">
-        <v>14</v>
-      </c>
+      <c r="B14" s="2"/>
       <c r="C14" t="s">
         <v>23</v>
       </c>
@@ -695,9 +693,7 @@
       <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="3">
-        <v>12</v>
-      </c>
+      <c r="B15" s="3"/>
       <c r="C15" t="s">
         <v>24</v>
       </c>
@@ -706,9 +702,7 @@
       <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="2">
-        <v>14</v>
-      </c>
+      <c r="B17" s="2"/>
       <c r="C17" t="s">
         <v>23</v>
       </c>
@@ -717,9 +711,7 @@
       <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="3">
-        <v>12</v>
-      </c>
+      <c r="B18" s="3"/>
       <c r="C18" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
İş türü - try catch yapıldı. koku testi eklendi. formül yazma şartı olarak adet yerine süre yapıldı.
</commit_message>
<xml_diff>
--- a/Config_and_Inputs/ConfigFile.xlsx
+++ b/Config_and_Inputs/ConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\can.sarihan\Documents\UiPath\Taslama_Surec_Otomasyonu\Config_and_Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FA6709-008C-40A6-B192-580561C31E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E603CEE7-8964-46A6-99EA-20721F7B27AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,7 +566,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,7 +641,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="2">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -652,7 +652,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="3">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -663,7 +663,7 @@
         <v>43</v>
       </c>
       <c r="B11" s="2">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -674,7 +674,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="3">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -684,7 +684,9 @@
       <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <v>27</v>
+      </c>
       <c r="C14" t="s">
         <v>23</v>
       </c>
@@ -693,7 +695,9 @@
       <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="3">
+        <v>27</v>
+      </c>
       <c r="C15" t="s">
         <v>24</v>
       </c>
@@ -702,7 +706,9 @@
       <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>27</v>
+      </c>
       <c r="C17" t="s">
         <v>23</v>
       </c>
@@ -711,7 +717,9 @@
       <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3">
+        <v>27</v>
+      </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>

</xml_diff>